<commit_message>
Atualização Mapeamento Conferência Purchase DW
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_Purchase_DW.xlsx
+++ b/Documentação/Planilhas/Conferencia_Purchase_DW.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="362">
   <si>
     <t>nr_cia</t>
   </si>
@@ -1127,10 +1127,19 @@
     <t>está nulo na view</t>
   </si>
   <si>
-    <t>NR_REFERENCIA_FISCAL</t>
-  </si>
-  <si>
-    <t>na det</t>
+    <t>Sessão "tdrecl504m00l". Fazer o detalhamento da Referência Fiscal desejada. Na aba superior Geral, seção "Dados Fiscais" verificar se "Origem da Mercadoria" é "Estrangeiro com Importação Direta" ou "Estrangeiro com Importação Direta-CAMEX". Se for, na aba inferior "Imposto por linha rec fiscal", pegar a informação da coluna "Valor" onde o Tipo de Imposto é PIS</t>
+  </si>
+  <si>
+    <t>Sessão "tdrecl504m00l". Fazer o detalhamento da Referência Fiscal desejada. Na aba superior Geral, seção "Dados Fiscais" verificar se "Origem da Mercadoria" é "Estrangeiro com Importação Direta" ou "Estrangeiro com Importação Direta-CAMEX". Se for, na aba inferior "Imposto por linha rec fiscal", pegar a informação da coluna "Valor" onde o Tipo de Imposto é COFINS</t>
+  </si>
+  <si>
+    <t>Sessão "tdrecl504m00l". Fazer o detalhamento da referência Fiscal desejada. Na aba inferior "Linhas" detalhar a linha apresentada. Na aba superior Geral, seção "Dados Fiscais" verificar se "Origem da Mercadoria" é "Estrangeiro com Importação Direta" ou "Estrangeiro com Importação Direta-CAMEX". Se for, na aba "Outros", seção "Despesas [Valores Rateados]"  pegar a informação de "Frete"</t>
+  </si>
+  <si>
+    <t>Sessão "tdrecl504m00l". Fazer o detalhamento da referência Fiscal desejada. Na aba inferior "Linhas" detalhar a linha apresentada. Na aba superior Geral, seção "Dados Fiscais" verificar se "Origem da Mercadoria" é "Estrangeiro com Importação Direta" ou "Estrangeiro com Importação Direta-CAMEX". Se for, na aba "Geral", seção "Dados de Compra"  pegar a informação de "Preço de Custo"</t>
+  </si>
+  <si>
+    <t>Não consegui mapear pelas telas do LN</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1211,8 +1220,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA7E7E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1261,11 +1276,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1287,6 +1320,30 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1299,32 +1356,17 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2042,9 +2084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L19" sqref="L19:L24"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3191,253 +3233,265 @@
       <c r="X17" s="3"/>
     </row>
     <row r="19" spans="1:24" ht="11.25" customHeight="1">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="L19" s="18" t="s">
+      <c r="L19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="N19" s="13" t="s">
+      <c r="N19" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="O19" s="13" t="s">
+      <c r="O19" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="P19" s="14" t="s">
+      <c r="P19" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="Q19" s="17" t="s">
+      <c r="Q19" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="R19" s="16" t="s">
+      <c r="R19" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="S19" s="10" t="s">
+      <c r="S19" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="T19" s="12" t="s">
+      <c r="T19" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="U19" s="13" t="s">
+      <c r="U19" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="V19" s="14" t="s">
+      <c r="V19" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="W19" s="15" t="s">
+      <c r="W19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="X19" s="11" t="s">
+      <c r="X19" s="19" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="12"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="11"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="19"/>
     </row>
     <row r="21" spans="1:24">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="11"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="18"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="19"/>
     </row>
     <row r="22" spans="1:24">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="11"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="19"/>
     </row>
     <row r="23" spans="1:24">
-      <c r="B23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="Q23" s="17"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="Q23" s="16"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="14"/>
       <c r="V23" s="6"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="11"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="19"/>
     </row>
     <row r="24" spans="1:24">
-      <c r="B24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="Q24" s="17"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="13"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="Q24" s="16"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="14"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="19"/>
     </row>
     <row r="25" spans="1:24">
-      <c r="B25" s="18"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="Q25" s="17"/>
+      <c r="B25" s="13"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="Q25" s="16"/>
       <c r="T25" s="6"/>
-      <c r="U25" s="13"/>
+      <c r="U25" s="14"/>
       <c r="V25" s="6"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="11"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="19"/>
     </row>
     <row r="26" spans="1:24">
-      <c r="B26" s="18"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="Q26" s="17"/>
+      <c r="B26" s="13"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="Q26" s="16"/>
       <c r="T26" s="6"/>
-      <c r="U26" s="13"/>
+      <c r="U26" s="14"/>
       <c r="V26" s="6"/>
-      <c r="W26" s="15"/>
+      <c r="W26" s="21"/>
     </row>
     <row r="27" spans="1:24">
-      <c r="B27" s="18"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="Q27" s="17"/>
+      <c r="B27" s="13"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="Q27" s="16"/>
       <c r="T27" s="6"/>
-      <c r="U27" s="13"/>
+      <c r="U27" s="14"/>
       <c r="V27" s="6"/>
-      <c r="W27" s="15"/>
+      <c r="W27" s="21"/>
     </row>
     <row r="28" spans="1:24">
-      <c r="B28" s="18"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="Q28" s="17"/>
+      <c r="B28" s="13"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="Q28" s="16"/>
       <c r="T28" s="6"/>
-      <c r="U28" s="13"/>
+      <c r="U28" s="14"/>
       <c r="V28" s="6"/>
-      <c r="W28" s="15"/>
+      <c r="W28" s="21"/>
     </row>
     <row r="29" spans="1:24">
-      <c r="B29" s="18"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="Q29" s="17"/>
+      <c r="B29" s="13"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="Q29" s="16"/>
       <c r="T29" s="6"/>
-      <c r="U29" s="13"/>
+      <c r="U29" s="14"/>
       <c r="V29" s="6"/>
-      <c r="W29" s="15"/>
+      <c r="W29" s="21"/>
     </row>
     <row r="30" spans="1:24">
-      <c r="Q30" s="17"/>
-      <c r="W30" s="15"/>
+      <c r="Q30" s="16"/>
+      <c r="W30" s="21"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="Q31" s="17"/>
-      <c r="W31" s="15"/>
+      <c r="Q31" s="16"/>
+      <c r="W31" s="21"/>
     </row>
     <row r="32" spans="1:24">
-      <c r="W32" s="15"/>
+      <c r="W32" s="21"/>
     </row>
     <row r="33" spans="17:23">
-      <c r="Q33" s="9" t="s">
+      <c r="Q33" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="W33" s="15"/>
+      <c r="W33" s="21"/>
     </row>
     <row r="34" spans="17:23">
-      <c r="Q34" s="9"/>
+      <c r="Q34" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="Q33:Q34"/>
+    <mergeCell ref="S19:S22"/>
+    <mergeCell ref="X19:X25"/>
+    <mergeCell ref="T19:T24"/>
+    <mergeCell ref="U19:U29"/>
+    <mergeCell ref="V19:V22"/>
+    <mergeCell ref="W19:W33"/>
+    <mergeCell ref="N19:N29"/>
+    <mergeCell ref="O19:O29"/>
+    <mergeCell ref="P19:P22"/>
+    <mergeCell ref="R19:R22"/>
+    <mergeCell ref="Q19:Q31"/>
     <mergeCell ref="M19:M24"/>
     <mergeCell ref="E19:E22"/>
     <mergeCell ref="D19:D22"/>
@@ -3449,18 +3503,6 @@
     <mergeCell ref="J19:J24"/>
     <mergeCell ref="K19:K24"/>
     <mergeCell ref="L19:L24"/>
-    <mergeCell ref="N19:N29"/>
-    <mergeCell ref="O19:O29"/>
-    <mergeCell ref="P19:P22"/>
-    <mergeCell ref="R19:R22"/>
-    <mergeCell ref="Q19:Q31"/>
-    <mergeCell ref="Q33:Q34"/>
-    <mergeCell ref="S19:S22"/>
-    <mergeCell ref="X19:X25"/>
-    <mergeCell ref="T19:T24"/>
-    <mergeCell ref="U19:U29"/>
-    <mergeCell ref="V19:V22"/>
-    <mergeCell ref="W19:W33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3469,17 +3511,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AR37"/>
+  <dimension ref="A1:AR34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN23" sqref="AN23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AQ25" sqref="AQ25:AQ33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="20" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="21" style="3" customWidth="1"/>
@@ -3510,146 +3552,146 @@
     <col min="33" max="33" width="22.85546875" style="3" customWidth="1"/>
     <col min="34" max="34" width="24.42578125" style="3" customWidth="1"/>
     <col min="35" max="35" width="25.28515625" style="3" customWidth="1"/>
-    <col min="36" max="36" width="15.7109375" style="3" customWidth="1"/>
-    <col min="37" max="37" width="20.140625" style="3" customWidth="1"/>
-    <col min="38" max="38" width="18.7109375" style="3" customWidth="1"/>
-    <col min="39" max="42" width="15.7109375" style="3" customWidth="1"/>
+    <col min="36" max="36" width="34.28515625" style="3" customWidth="1"/>
+    <col min="37" max="37" width="31.7109375" style="3" customWidth="1"/>
+    <col min="38" max="39" width="33.85546875" style="3" customWidth="1"/>
+    <col min="40" max="42" width="15.7109375" style="3" customWidth="1"/>
     <col min="43" max="43" width="42.140625" style="3" customWidth="1"/>
     <col min="44" max="44" width="26.140625" style="3" customWidth="1"/>
     <col min="45" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="W1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Y1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="Z1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="AA1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AB1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AC1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="AD1" s="20" t="s">
+      <c r="AD1" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="AE1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AF1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="AG1" s="20" t="s">
+      <c r="AG1" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="AH1" s="20" t="s">
+      <c r="AH1" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="AI1" s="20" t="s">
+      <c r="AI1" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="AJ1" s="20" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="AK1" s="20" t="s">
+      <c r="AK1" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="AL1" s="20" t="s">
+      <c r="AL1" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="AM1" s="20" t="s">
+      <c r="AM1" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="AN1" s="20" t="s">
+      <c r="AN1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="AO1" s="20" t="s">
+      <c r="AO1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="AP1" s="20" t="s">
+      <c r="AP1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="AQ1" s="20" t="s">
+      <c r="AQ1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="AR1" s="20" t="s">
+      <c r="AR1" s="10" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5045,7 +5087,7 @@
       <c r="Q12" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="R12" s="19" t="s">
+      <c r="R12" s="9" t="s">
         <v>322</v>
       </c>
       <c r="S12" s="3" t="s">
@@ -6468,412 +6510,502 @@
       </c>
     </row>
     <row r="25" spans="1:44" ht="11.25" customHeight="1">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="13" t="s">
         <v>324</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="J25" s="18" t="s">
+      <c r="J25" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="L25" s="18" t="s">
+      <c r="L25" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="N25" s="18" t="s">
+      <c r="N25" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="O25" s="18" t="s">
+      <c r="O25" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="P25" s="18" t="s">
+      <c r="P25" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="Q25" s="17" t="s">
+      <c r="Q25" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="R25" s="17" t="s">
+      <c r="R25" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="S25" s="17" t="s">
+      <c r="S25" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="T25" s="17" t="s">
+      <c r="T25" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="U25" s="17" t="s">
+      <c r="U25" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="V25" s="17" t="s">
+      <c r="V25" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="W25" s="17" t="s">
+      <c r="W25" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="X25" s="17" t="s">
+      <c r="X25" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="Y25" s="17" t="s">
+      <c r="Y25" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="Z25" s="17" t="s">
+      <c r="Z25" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="AA25" s="11" t="s">
+      <c r="AA25" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="AC25" s="11" t="s">
+      <c r="AB25" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="AD25" s="11" t="s">
+      <c r="AC25" s="19" t="s">
         <v>356</v>
       </c>
-      <c r="AE25" s="18" t="s">
+      <c r="AD25" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="AE25" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="AF25" s="17" t="s">
+      <c r="AF25" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="AG25" s="17" t="s">
+      <c r="AG25" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="AH25" s="17" t="s">
+      <c r="AH25" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="AI25" s="17" t="s">
+      <c r="AI25" s="16" t="s">
         <v>350</v>
       </c>
-      <c r="AQ25" s="17" t="s">
+      <c r="AJ25" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="AK25" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="AL25" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="AM25" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="AN25" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="AO25" s="23"/>
+      <c r="AP25" s="24"/>
+      <c r="AQ25" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="AR25" s="17" t="s">
+      <c r="AR25" s="16" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="26" spans="1:44">
-      <c r="B26" s="17"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="17"/>
-      <c r="U26" s="17"/>
-      <c r="V26" s="17"/>
-      <c r="W26" s="17"/>
-      <c r="X26" s="17"/>
-      <c r="Y26" s="17"/>
-      <c r="Z26" s="17"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="AC26" s="11"/>
-      <c r="AD26" s="11"/>
-      <c r="AE26" s="18"/>
-      <c r="AF26" s="17"/>
-      <c r="AG26" s="17"/>
-      <c r="AH26" s="17"/>
-      <c r="AI26" s="17"/>
-      <c r="AQ26" s="17"/>
-      <c r="AR26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="13"/>
+      <c r="AF26" s="16"/>
+      <c r="AG26" s="16"/>
+      <c r="AH26" s="16"/>
+      <c r="AI26" s="16"/>
+      <c r="AJ26" s="16"/>
+      <c r="AK26" s="16"/>
+      <c r="AL26" s="16"/>
+      <c r="AM26" s="16"/>
+      <c r="AN26" s="22"/>
+      <c r="AO26" s="23"/>
+      <c r="AP26" s="24"/>
+      <c r="AQ26" s="16"/>
+      <c r="AR26" s="16"/>
     </row>
     <row r="27" spans="1:44">
-      <c r="B27" s="17"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="17"/>
-      <c r="V27" s="17"/>
-      <c r="W27" s="17"/>
-      <c r="X27" s="17"/>
-      <c r="Y27" s="17"/>
-      <c r="Z27" s="17"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="18"/>
-      <c r="AF27" s="17"/>
-      <c r="AG27" s="17"/>
-      <c r="AH27" s="17"/>
-      <c r="AI27" s="17"/>
-      <c r="AQ27" s="17"/>
-      <c r="AR27" s="17"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="16"/>
+      <c r="AG27" s="16"/>
+      <c r="AH27" s="16"/>
+      <c r="AI27" s="16"/>
+      <c r="AJ27" s="16"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="16"/>
+      <c r="AM27" s="16"/>
+      <c r="AN27" s="22"/>
+      <c r="AO27" s="23"/>
+      <c r="AP27" s="24"/>
+      <c r="AQ27" s="16"/>
+      <c r="AR27" s="16"/>
     </row>
     <row r="28" spans="1:44">
-      <c r="B28" s="17"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
-      <c r="S28" s="17"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="17"/>
-      <c r="V28" s="17"/>
-      <c r="W28" s="17"/>
-      <c r="X28" s="17"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="17"/>
-      <c r="AA28" s="11"/>
-      <c r="AC28" s="11"/>
-      <c r="AD28" s="11"/>
-      <c r="AE28" s="18"/>
-      <c r="AF28" s="17"/>
-      <c r="AG28" s="17"/>
-      <c r="AH28" s="17"/>
-      <c r="AI28" s="17"/>
-      <c r="AQ28" s="17"/>
-      <c r="AR28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="13"/>
+      <c r="AF28" s="16"/>
+      <c r="AG28" s="16"/>
+      <c r="AH28" s="16"/>
+      <c r="AI28" s="16"/>
+      <c r="AJ28" s="16"/>
+      <c r="AK28" s="16"/>
+      <c r="AL28" s="16"/>
+      <c r="AM28" s="16"/>
+      <c r="AN28" s="22"/>
+      <c r="AO28" s="23"/>
+      <c r="AP28" s="24"/>
+      <c r="AQ28" s="16"/>
+      <c r="AR28" s="16"/>
     </row>
     <row r="29" spans="1:44">
-      <c r="B29" s="17"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17"/>
-      <c r="W29" s="17"/>
-      <c r="X29" s="17"/>
-      <c r="Y29" s="17"/>
-      <c r="Z29" s="17"/>
-      <c r="AA29" s="11"/>
-      <c r="AC29" s="11"/>
-      <c r="AD29" s="11"/>
-      <c r="AE29" s="18"/>
-      <c r="AF29" s="17"/>
-      <c r="AG29" s="17"/>
-      <c r="AH29" s="17"/>
-      <c r="AI29" s="17"/>
-      <c r="AQ29" s="17"/>
-      <c r="AR29" s="17"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="13"/>
+      <c r="AF29" s="16"/>
+      <c r="AG29" s="16"/>
+      <c r="AH29" s="16"/>
+      <c r="AI29" s="16"/>
+      <c r="AJ29" s="16"/>
+      <c r="AK29" s="16"/>
+      <c r="AL29" s="16"/>
+      <c r="AM29" s="16"/>
+      <c r="AN29" s="22"/>
+      <c r="AO29" s="23"/>
+      <c r="AP29" s="24"/>
+      <c r="AQ29" s="16"/>
+      <c r="AR29" s="16"/>
     </row>
     <row r="30" spans="1:44">
-      <c r="B30" s="17"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="11"/>
-      <c r="AC30" s="11"/>
-      <c r="AD30" s="11"/>
-      <c r="AE30" s="18"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="17"/>
-      <c r="AI30" s="17"/>
-      <c r="AQ30" s="17"/>
-      <c r="AR30" s="17"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="16"/>
+      <c r="Y30" s="16"/>
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
+      <c r="AE30" s="13"/>
+      <c r="AF30" s="16"/>
+      <c r="AG30" s="16"/>
+      <c r="AH30" s="16"/>
+      <c r="AI30" s="16"/>
+      <c r="AJ30" s="16"/>
+      <c r="AK30" s="16"/>
+      <c r="AL30" s="16"/>
+      <c r="AM30" s="16"/>
+      <c r="AN30" s="22"/>
+      <c r="AO30" s="23"/>
+      <c r="AP30" s="24"/>
+      <c r="AQ30" s="16"/>
+      <c r="AR30" s="16"/>
     </row>
     <row r="31" spans="1:44">
-      <c r="B31" s="17"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
-      <c r="V31" s="17"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="17"/>
-      <c r="Y31" s="17"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="11"/>
-      <c r="AC31" s="11"/>
-      <c r="AD31" s="11"/>
-      <c r="AE31" s="18"/>
-      <c r="AF31" s="17"/>
-      <c r="AG31" s="17"/>
-      <c r="AH31" s="17"/>
-      <c r="AI31" s="17"/>
-      <c r="AQ31" s="17"/>
-      <c r="AR31" s="17"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="16"/>
+      <c r="Z31" s="16"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="13"/>
+      <c r="AF31" s="16"/>
+      <c r="AG31" s="16"/>
+      <c r="AH31" s="16"/>
+      <c r="AI31" s="16"/>
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="16"/>
+      <c r="AL31" s="16"/>
+      <c r="AM31" s="16"/>
+      <c r="AN31" s="22"/>
+      <c r="AO31" s="23"/>
+      <c r="AP31" s="24"/>
+      <c r="AQ31" s="16"/>
+      <c r="AR31" s="16"/>
     </row>
     <row r="32" spans="1:44">
-      <c r="B32" s="17"/>
-      <c r="J32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="17"/>
-      <c r="AA32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="18"/>
-      <c r="AF32" s="17"/>
-      <c r="AG32" s="17"/>
-      <c r="AH32" s="17"/>
-      <c r="AI32" s="17"/>
-      <c r="AQ32" s="17"/>
-      <c r="AR32" s="17"/>
-    </row>
-    <row r="33" spans="2:44">
-      <c r="B33" s="17"/>
-      <c r="F33" s="21" t="s">
+      <c r="J32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="16"/>
+      <c r="Z32" s="16"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="13"/>
+      <c r="AF32" s="16"/>
+      <c r="AG32" s="16"/>
+      <c r="AH32" s="16"/>
+      <c r="AI32" s="16"/>
+      <c r="AJ32" s="16"/>
+      <c r="AK32" s="16"/>
+      <c r="AL32" s="16"/>
+      <c r="AM32" s="16"/>
+      <c r="AN32" s="22"/>
+      <c r="AO32" s="23"/>
+      <c r="AP32" s="24"/>
+      <c r="AQ32" s="16"/>
+      <c r="AR32" s="16"/>
+    </row>
+    <row r="33" spans="6:44">
+      <c r="F33" s="11" t="s">
         <v>353</v>
       </c>
-      <c r="J33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="17"/>
-      <c r="V33" s="17"/>
-      <c r="W33" s="17"/>
-      <c r="X33" s="17"/>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="17"/>
-      <c r="AA33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="18"/>
-      <c r="AF33" s="17"/>
-      <c r="AG33" s="17"/>
-      <c r="AH33" s="17"/>
-      <c r="AI33" s="17"/>
-      <c r="AQ33" s="17"/>
-      <c r="AR33" s="17"/>
-    </row>
-    <row r="34" spans="2:44" ht="101.25">
-      <c r="B34" s="17"/>
+      <c r="J33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
+      <c r="AC33" s="19"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="13"/>
+      <c r="AF33" s="16"/>
+      <c r="AG33" s="16"/>
+      <c r="AH33" s="16"/>
+      <c r="AI33" s="16"/>
+      <c r="AJ33" s="16"/>
+      <c r="AK33" s="16"/>
+      <c r="AL33" s="16"/>
+      <c r="AM33" s="16"/>
+      <c r="AN33" s="22"/>
+      <c r="AO33" s="23"/>
+      <c r="AP33" s="24"/>
+      <c r="AQ33" s="16"/>
+      <c r="AR33" s="16"/>
+    </row>
+    <row r="34" spans="6:44" ht="101.25">
       <c r="F34" s="8" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="35" spans="2:44">
-      <c r="B35" s="17"/>
-    </row>
-    <row r="36" spans="2:44">
-      <c r="B36" s="17"/>
-    </row>
-    <row r="37" spans="2:44">
-      <c r="B37" s="17"/>
-    </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="40">
+    <mergeCell ref="AM25:AM33"/>
+    <mergeCell ref="AB25:AB33"/>
+    <mergeCell ref="AN25:AP33"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="AK25:AK33"/>
+    <mergeCell ref="AL25:AL33"/>
+    <mergeCell ref="AJ25:AJ33"/>
+    <mergeCell ref="K25:K31"/>
+    <mergeCell ref="L25:L33"/>
+    <mergeCell ref="N25:N33"/>
+    <mergeCell ref="E25:E31"/>
+    <mergeCell ref="C25:C31"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="G25:G31"/>
+    <mergeCell ref="I25:I31"/>
+    <mergeCell ref="J25:J33"/>
+    <mergeCell ref="R25:R33"/>
+    <mergeCell ref="W25:W33"/>
+    <mergeCell ref="X25:X33"/>
+    <mergeCell ref="Y25:Y33"/>
+    <mergeCell ref="O25:O33"/>
+    <mergeCell ref="P25:P33"/>
+    <mergeCell ref="Q25:Q33"/>
+    <mergeCell ref="T25:T33"/>
+    <mergeCell ref="U25:U33"/>
     <mergeCell ref="AH25:AH33"/>
     <mergeCell ref="AR25:AR33"/>
     <mergeCell ref="S25:S33"/>
     <mergeCell ref="AI25:AI33"/>
-    <mergeCell ref="B25:B37"/>
     <mergeCell ref="H25:H31"/>
     <mergeCell ref="F25:F31"/>
     <mergeCell ref="AQ25:AQ33"/>
@@ -6885,24 +7017,6 @@
     <mergeCell ref="AF25:AF33"/>
     <mergeCell ref="AG25:AG33"/>
     <mergeCell ref="V25:V33"/>
-    <mergeCell ref="R25:R33"/>
-    <mergeCell ref="W25:W33"/>
-    <mergeCell ref="X25:X33"/>
-    <mergeCell ref="Y25:Y33"/>
-    <mergeCell ref="O25:O33"/>
-    <mergeCell ref="P25:P33"/>
-    <mergeCell ref="Q25:Q33"/>
-    <mergeCell ref="T25:T33"/>
-    <mergeCell ref="U25:U33"/>
-    <mergeCell ref="K25:K31"/>
-    <mergeCell ref="L25:L33"/>
-    <mergeCell ref="N25:N33"/>
-    <mergeCell ref="E25:E31"/>
-    <mergeCell ref="C25:C31"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="G25:G31"/>
-    <mergeCell ref="I25:I31"/>
-    <mergeCell ref="J25:J33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>